<commit_message>
Exam Screen and Exam time
</commit_message>
<xml_diff>
--- a/student_upload - 5000.xlsx
+++ b/student_upload - 5000.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="146">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -587,10 +587,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -657,7 +657,7 @@
         <v>9876543210</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -683,7 +683,7 @@
         <v>9876543211</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -709,12 +709,12 @@
         <v>9876543212</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
@@ -735,12 +735,12 @@
         <v>9876543213</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -761,12 +761,12 @@
         <v>9876543214</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>19</v>
@@ -787,12 +787,12 @@
         <v>9876543215</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
@@ -813,12 +813,12 @@
         <v>9876543216</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>14</v>
@@ -839,7 +839,7 @@
         <v>9876543217</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -865,12 +865,12 @@
         <v>9876543218</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
@@ -891,12 +891,12 @@
         <v>9876543219</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>14</v>
@@ -917,12 +917,12 @@
         <v>9876543220</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -943,12 +943,12 @@
         <v>9876543221</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>19</v>
@@ -969,12 +969,12 @@
         <v>9876543222</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
@@ -995,7 +995,7 @@
         <v>9876543223</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
@@ -1021,12 +1021,12 @@
         <v>9876543224</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
@@ -1047,12 +1047,12 @@
         <v>9876543225</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>19</v>
@@ -1073,12 +1073,12 @@
         <v>9876543226</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>9</v>
@@ -1099,12 +1099,12 @@
         <v>9876543227</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>14</v>
@@ -1125,12 +1125,12 @@
         <v>9876543228</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>19</v>
@@ -1151,12 +1151,12 @@
         <v>9876543229</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
@@ -1177,7 +1177,7 @@
         <v>9876543230</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>76</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>9876543231</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>9876543232</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>82</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>9876543233</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>85</v>
       </c>
@@ -1281,12 +1281,12 @@
         <v>9876543234</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
@@ -1307,12 +1307,12 @@
         <v>9876543235</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>14</v>
@@ -1333,12 +1333,12 @@
         <v>9876543236</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>19</v>
@@ -1359,12 +1359,12 @@
         <v>9876543237</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B30" s="5" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>9</v>
@@ -1385,7 +1385,7 @@
         <v>9876543238</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>100</v>
       </c>
@@ -1411,12 +1411,12 @@
         <v>9876543239</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B32" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
@@ -1437,12 +1437,12 @@
         <v>9876543210</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>14</v>
@@ -1463,12 +1463,12 @@
         <v>9876543211</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>19</v>
@@ -1489,12 +1489,12 @@
         <v>9876543212</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>9</v>
@@ -1515,12 +1515,12 @@
         <v>9876543213</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>14</v>
@@ -1541,12 +1541,12 @@
         <v>9876543214</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>19</v>
@@ -1567,12 +1567,12 @@
         <v>9876543215</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B38" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
@@ -1593,7 +1593,7 @@
         <v>9876543216</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>110</v>
       </c>
@@ -1619,12 +1619,12 @@
         <v>9876543217</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>19</v>
@@ -1645,12 +1645,12 @@
         <v>9876543218</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B41" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>9</v>
@@ -1671,12 +1671,12 @@
         <v>9876543219</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B42" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>14</v>
@@ -1697,12 +1697,12 @@
         <v>9876543220</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B43" s="5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>9</v>
@@ -1723,12 +1723,12 @@
         <v>9876543221</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B44" s="5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>19</v>
@@ -1749,12 +1749,12 @@
         <v>9876543222</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B45" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>14</v>
@@ -1775,12 +1775,12 @@
         <v>9876543223</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B46" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>9</v>
@@ -1801,12 +1801,12 @@
         <v>9876543224</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B47" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>14</v>
@@ -1827,12 +1827,12 @@
         <v>9876543225</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B48" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>19</v>
@@ -1853,12 +1853,12 @@
         <v>9876543226</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B49" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>9</v>
@@ -1879,12 +1879,12 @@
         <v>9876543227</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B50" s="5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>14</v>
@@ -1905,12 +1905,12 @@
         <v>9876543228</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B51" s="5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>19</v>
@@ -1931,12 +1931,12 @@
         <v>9876543229</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B52" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>9</v>
@@ -1957,12 +1957,12 @@
         <v>9876543230</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B53" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>14</v>
@@ -1983,12 +1983,12 @@
         <v>9876543231</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B54" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>19</v>
@@ -2009,12 +2009,12 @@
         <v>9876543232</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B55" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>9</v>
@@ -2035,12 +2035,12 @@
         <v>9876543233</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B56" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>14</v>
@@ -2061,12 +2061,12 @@
         <v>9876543234</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B57" s="5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>9</v>
@@ -2087,12 +2087,12 @@
         <v>9876543235</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B58" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>14</v>
@@ -2113,12 +2113,12 @@
         <v>9876543236</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B59" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>19</v>
@@ -2139,12 +2139,12 @@
         <v>9876543237</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B60" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>9</v>
@@ -2165,12 +2165,12 @@
         <v>9876543238</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B61" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>19</v>
@@ -2191,12 +2191,12 @@
         <v>9876543239</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B62" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>9</v>
@@ -2217,12 +2217,12 @@
         <v>9876543210</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B63" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>14</v>
@@ -2243,12 +2243,12 @@
         <v>9876543211</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B64" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>19</v>
@@ -2269,7 +2269,7 @@
         <v>9876543212</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
         <v>136</v>
       </c>
@@ -2295,12 +2295,12 @@
         <v>9876543213</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B66" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>14</v>
@@ -2321,12 +2321,12 @@
         <v>9876543214</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B67" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>19</v>
@@ -2347,12 +2347,12 @@
         <v>9876543215</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B68" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>9</v>
@@ -2373,12 +2373,12 @@
         <v>9876543216</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B69" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>14</v>
@@ -2399,12 +2399,12 @@
         <v>9876543217</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B70" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>19</v>
@@ -2425,12 +2425,12 @@
         <v>9876543218</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B71" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>9</v>
@@ -2451,7 +2451,7 @@
         <v>9876543219</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
         <v>143</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>9876543220</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
         <v>144</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>9876543221</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
         <v>145</v>
       </c>
@@ -2527,6 +2527,292 @@
       </c>
       <c r="H74" s="5" t="n">
         <v>9876543222</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="6" t="n">
+        <v>40238</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H75" s="5" t="n">
+        <v>9876543223</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="6" t="n">
+        <v>41219</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="5" t="n">
+        <v>9876543224</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="6" t="n">
+        <v>41356</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="5" t="n">
+        <v>9876543225</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="6" t="n">
+        <v>40775</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H78" s="5" t="n">
+        <v>9876543226</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="6" t="n">
+        <v>41091</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <v>9876543227</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B80" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="6" t="n">
+        <v>40278</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <v>9876543228</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="6" t="n">
+        <v>41560</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H81" s="5" t="n">
+        <v>9876543229</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="6" t="n">
+        <v>40924</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H82" s="5" t="n">
+        <v>9876543230</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="6" t="n">
+        <v>40733</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H83" s="5" t="n">
+        <v>9876543231</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B84" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" s="6" t="n">
+        <v>40239</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H84" s="5" t="n">
+        <v>9876543232</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="6" t="n">
+        <v>41220</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H85" s="5" t="n">
+        <v>9876543233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>